<commit_message>
creacion de codigo para SD
</commit_message>
<xml_diff>
--- a/Pinout PROYECTO 2.xlsx
+++ b/Pinout PROYECTO 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\PROYECTO 2\PROYECTO_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B53750-9A66-42B8-9C5B-02EB3F5DB95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9414066A-C1FC-4FF4-898B-2CA1E7F49323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="127">
   <si>
     <t>Entradas</t>
   </si>
@@ -132,27 +132,6 @@
     <t>RS</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>GPIO 32</t>
-  </si>
-  <si>
-    <t>GPIO 33</t>
-  </si>
-  <si>
-    <t>GPIO 25</t>
-  </si>
-  <si>
-    <t>GPIO 26</t>
-  </si>
-  <si>
-    <t>GPIO 27</t>
-  </si>
-  <si>
-    <t>GPIO 14</t>
-  </si>
-  <si>
     <t>GPIO13</t>
   </si>
   <si>
@@ -270,24 +249,6 @@
     <t>PF4</t>
   </si>
   <si>
-    <t>VOLTAJE RED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENVIO </t>
-  </si>
-  <si>
-    <t>RECIBO</t>
-  </si>
-  <si>
-    <t>ENVIO</t>
-  </si>
-  <si>
-    <t>TX2</t>
-  </si>
-  <si>
-    <t>RX2</t>
-  </si>
-  <si>
     <t>ENTRADAS</t>
   </si>
   <si>
@@ -309,7 +270,142 @@
     <t>J4</t>
   </si>
   <si>
-    <t>VOLTAJE AZUL</t>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Echo </t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>PD_2</t>
+  </si>
+  <si>
+    <t>PF_4</t>
+  </si>
+  <si>
+    <t>PF_0</t>
+  </si>
+  <si>
+    <t>PE_4</t>
+  </si>
+  <si>
+    <t>BUZZER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF_2 </t>
+  </si>
+  <si>
+    <t>Echo</t>
+  </si>
+  <si>
+    <t>HMOSI</t>
+  </si>
+  <si>
+    <t>HMISO</t>
+  </si>
+  <si>
+    <t>HSCK</t>
+  </si>
+  <si>
+    <t>HCS</t>
+  </si>
+  <si>
+    <t>GPIO12</t>
+  </si>
+  <si>
+    <t>GPIO14</t>
+  </si>
+  <si>
+    <t>GPIO15</t>
+  </si>
+  <si>
+    <t>VMOSI</t>
+  </si>
+  <si>
+    <t>VMISO</t>
+  </si>
+  <si>
+    <t>VSCK</t>
+  </si>
+  <si>
+    <t>VCS</t>
+  </si>
+  <si>
+    <t>GPIO23</t>
+  </si>
+  <si>
+    <t>GPIO19</t>
+  </si>
+  <si>
+    <t>GPIO18</t>
+  </si>
+  <si>
+    <t>GPIO5</t>
+  </si>
+  <si>
+    <t>GPIO32</t>
+  </si>
+  <si>
+    <t>GPIO33</t>
+  </si>
+  <si>
+    <t>GPIO25</t>
+  </si>
+  <si>
+    <t>GPIO26</t>
+  </si>
+  <si>
+    <t>GPIO27</t>
+  </si>
+  <si>
+    <t>GPIO22</t>
+  </si>
+  <si>
+    <t>GPIO21</t>
+  </si>
+  <si>
+    <t>GPIO4</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS </t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>GPIO1</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>GPIO17</t>
+  </si>
+  <si>
+    <t>GPIO16</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
   </si>
 </sst>
 </file>
@@ -341,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,19 +452,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,6 +471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -427,7 +517,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -436,22 +525,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65D1A52-722E-4D88-830B-F2F29FFF5A54}">
   <dimension ref="A3:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,17 +1206,19 @@
       <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="16" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1131,16 +1227,18 @@
       <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="4"/>
+      <c r="B5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1149,15 +1247,18 @@
       <c r="I5" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J5" s="24" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="B6" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1166,9 +1267,18 @@
       <c r="I6" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="J6" s="24" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E7" s="4"/>
+      <c r="B7" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1177,11 +1287,19 @@
       <c r="I7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E8" s="10" t="s">
-        <v>25</v>
+      <c r="B8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -1191,11 +1309,19 @@
       <c r="I8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="16" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E9" s="9" t="s">
-        <v>8</v>
+      <c r="B9" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>11</v>
@@ -1205,17 +1331,19 @@
       <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="J9" s="21" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>32</v>
+      <c r="B10" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -1225,17 +1353,20 @@
       <c r="I10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J10" s="21" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>33</v>
+      <c r="A11" s="7"/>
+      <c r="B11" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
@@ -1245,20 +1376,19 @@
       <c r="I11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>84</v>
+      <c r="J11" s="23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>34</v>
+      <c r="B12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>14</v>
@@ -1268,20 +1398,16 @@
       <c r="I12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>83</v>
+      <c r="J12" s="23" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>35</v>
+      <c r="A13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="E13" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
@@ -1291,18 +1417,16 @@
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="22" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>81</v>
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>16</v>
@@ -1312,16 +1436,16 @@
       <c r="I14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="22" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="E15" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1330,15 +1454,17 @@
       <c r="I15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>41</v>
+      <c r="A16" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>4</v>
@@ -1350,12 +1476,12 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>85</v>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>3</v>
@@ -1367,393 +1493,483 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B39" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
+      <c r="B40" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L45" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="M45" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="N45" t="s">
+        <v>79</v>
+      </c>
+      <c r="O45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N46" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="1"/>
-      <c r="D45" t="s">
+      <c r="O46" s="14"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E45" t="s">
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M47" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M48" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M49" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D50" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F45" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="L45" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="M45" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="N45" t="s">
-        <v>92</v>
-      </c>
-      <c r="O45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="15" t="s">
+      <c r="F50" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G50" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L46" s="15" t="s">
+      <c r="L50" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="M46" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="15" t="s">
+      <c r="M50" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G47" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L47" s="15" t="s">
+      <c r="G51" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M51" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="M47" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G48" s="15" t="s">
+      <c r="N51" s="18"/>
+      <c r="O51" s="14"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="L48" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="M48" s="15" t="s">
+      <c r="L52" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="G49" s="15" t="s">
+      <c r="M52" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N52" s="18"/>
+      <c r="O52" s="14"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="L49" s="15" t="s">
+      <c r="G53" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="M53" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="M49" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G50" s="15" t="s">
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G54" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="L50" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="M50" s="15" t="s">
+      <c r="L54" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="N50" s="17"/>
-      <c r="O50" s="17"/>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G51" s="15" t="s">
+      <c r="M54" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L51" s="15" t="s">
+      <c r="G55" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M55" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="M51" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="N51" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="O51" s="17"/>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L52" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="M52" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="N52" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="O52" s="17"/>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="L53" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="M53" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="N53" s="17"/>
-      <c r="O53" s="17"/>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L54" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="M54" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="L55" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="M55" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prueba de sensor en tiva C
Se esta probando que el sensor sirva en la tiva C
</commit_message>
<xml_diff>
--- a/Pinout PROYECTO 2.xlsx
+++ b/Pinout PROYECTO 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\PROYECTO 2\PROYECTO_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA219984-CA8B-4AEE-9AE9-A19ECE64F1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA94D11-06EE-478C-89AA-422164C99CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="132">
   <si>
     <t>Entradas</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>PA_2</t>
+  </si>
+  <si>
+    <t>PE_0</t>
   </si>
 </sst>
 </file>
@@ -555,9 +558,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -566,6 +566,9 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65D1A52-722E-4D88-830B-F2F29FFF5A54}">
-  <dimension ref="A3:O64"/>
+  <dimension ref="A3:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1229,10 +1232,10 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1417,10 +1420,10 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="20"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1592,8 +1595,12 @@
       <c r="M40" s="9"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="L41" s="9"/>
@@ -1688,7 +1695,7 @@
       <c r="C47" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="24" t="s">
         <v>112</v>
       </c>
       <c r="E47" s="12"/>
@@ -1705,7 +1712,7 @@
         <v>52</v>
       </c>
       <c r="N47" s="12"/>
-      <c r="O47" s="25" t="s">
+      <c r="O47" s="24" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1716,10 +1723,10 @@
       <c r="C48" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="22" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="10" t="s">
@@ -1734,10 +1741,12 @@
       <c r="M48" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="N48" s="25" t="s">
+      <c r="N48" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="O48" s="12"/>
+      <c r="O48" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
@@ -1746,10 +1755,10 @@
       <c r="C49" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="23" t="s">
         <v>98</v>
       </c>
       <c r="F49" s="10" t="s">
@@ -1764,7 +1773,9 @@
       <c r="M49" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="O49" s="12"/>
+      <c r="O49" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
@@ -1774,7 +1785,7 @@
         <v>104</v>
       </c>
       <c r="D50" s="19"/>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="23" t="s">
         <v>99</v>
       </c>
       <c r="F50" s="10" t="s">
@@ -1799,7 +1810,7 @@
         <v>105</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="24" t="s">
+      <c r="E51" s="23" t="s">
         <v>100</v>
       </c>
       <c r="F51" s="10" t="s">
@@ -1817,7 +1828,7 @@
       <c r="N51" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="O51" s="25" t="s">
+      <c r="O51" s="24" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1828,10 +1839,10 @@
       <c r="C52" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="D52" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="24" t="s">
+      <c r="E52" s="23" t="s">
         <v>101</v>
       </c>
       <c r="F52" s="10" t="s">
@@ -1849,18 +1860,18 @@
       <c r="N52" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="O52" s="25" t="s">
+      <c r="O52" s="24" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D53" s="27" t="s">
         <v>125</v>
       </c>
       <c r="E53" s="12"/>
@@ -1877,15 +1888,15 @@
         <v>64</v>
       </c>
       <c r="N53" s="12"/>
-      <c r="O53" s="28" t="s">
+      <c r="O53" s="27" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="21" t="s">
         <v>116</v>
       </c>
       <c r="D54" s="12"/>
@@ -1903,15 +1914,15 @@
         <v>67</v>
       </c>
       <c r="N54" s="12"/>
-      <c r="O54" s="28" t="s">
+      <c r="O54" s="27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="21" t="s">
         <v>117</v>
       </c>
       <c r="D55" s="12"/>
@@ -1929,15 +1940,15 @@
         <v>68</v>
       </c>
       <c r="N55" s="12"/>
-      <c r="O55" s="28" t="s">
+      <c r="O55" s="27" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="21" t="s">
         <v>118</v>
       </c>
       <c r="F56" s="9"/>
@@ -1946,10 +1957,10 @@
       <c r="M56" s="9"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="21" t="s">
         <v>119</v>
       </c>
       <c r="F57" s="9"/>
@@ -1958,10 +1969,10 @@
       <c r="M57" s="9"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F58" s="9"/>
@@ -1970,10 +1981,10 @@
       <c r="M58" s="9"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="22" t="s">
+      <c r="C59" s="21" t="s">
         <v>121</v>
       </c>
       <c r="F59" s="9"/>
@@ -1982,43 +1993,51 @@
       <c r="M59" s="9"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="21" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="27" t="s">
+      <c r="C61" s="26" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="C62" s="26" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B63" s="26" t="s">
+      <c r="B63" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="C63" s="26" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="C64" s="26" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Prueba de sensor en tiva C"
This reverts commit 574c494eb14a1a260ea821e1e936d0351ebfce2c.
</commit_message>
<xml_diff>
--- a/Pinout PROYECTO 2.xlsx
+++ b/Pinout PROYECTO 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\PROYECTO 2\PROYECTO_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA94D11-06EE-478C-89AA-422164C99CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA219984-CA8B-4AEE-9AE9-A19ECE64F1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
   <si>
     <t>Entradas</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>PA_2</t>
-  </si>
-  <si>
-    <t>PE_0</t>
   </si>
 </sst>
 </file>
@@ -558,6 +555,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -566,9 +566,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1208,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65D1A52-722E-4D88-830B-F2F29FFF5A54}">
-  <dimension ref="A3:O65"/>
+  <dimension ref="A3:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,10 +1229,10 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1420,10 +1417,10 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1595,12 +1592,8 @@
       <c r="M40" s="9"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>80</v>
-      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="L41" s="9"/>
@@ -1695,7 +1688,7 @@
       <c r="C47" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="D47" s="25" t="s">
         <v>112</v>
       </c>
       <c r="E47" s="12"/>
@@ -1712,7 +1705,7 @@
         <v>52</v>
       </c>
       <c r="N47" s="12"/>
-      <c r="O47" s="24" t="s">
+      <c r="O47" s="25" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1723,10 +1716,10 @@
       <c r="C48" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="23" t="s">
         <v>97</v>
       </c>
       <c r="F48" s="10" t="s">
@@ -1741,12 +1734,10 @@
       <c r="M48" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="N48" s="24" t="s">
+      <c r="N48" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="O48" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="O48" s="12"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
@@ -1755,10 +1746,10 @@
       <c r="C49" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D49" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="24" t="s">
         <v>98</v>
       </c>
       <c r="F49" s="10" t="s">
@@ -1773,9 +1764,7 @@
       <c r="M49" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="O49" s="8" t="s">
-        <v>86</v>
-      </c>
+      <c r="O49" s="12"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
@@ -1785,7 +1774,7 @@
         <v>104</v>
       </c>
       <c r="D50" s="19"/>
-      <c r="E50" s="23" t="s">
+      <c r="E50" s="24" t="s">
         <v>99</v>
       </c>
       <c r="F50" s="10" t="s">
@@ -1810,7 +1799,7 @@
         <v>105</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="24" t="s">
         <v>100</v>
       </c>
       <c r="F51" s="10" t="s">
@@ -1828,7 +1817,7 @@
       <c r="N51" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="O51" s="24" t="s">
+      <c r="O51" s="25" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1839,10 +1828,10 @@
       <c r="C52" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="23" t="s">
+      <c r="E52" s="24" t="s">
         <v>101</v>
       </c>
       <c r="F52" s="10" t="s">
@@ -1860,18 +1849,18 @@
       <c r="N52" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="O52" s="24" t="s">
+      <c r="O52" s="25" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="27" t="s">
+      <c r="D53" s="28" t="s">
         <v>125</v>
       </c>
       <c r="E53" s="12"/>
@@ -1888,15 +1877,15 @@
         <v>64</v>
       </c>
       <c r="N53" s="12"/>
-      <c r="O53" s="27" t="s">
+      <c r="O53" s="28" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="22" t="s">
         <v>116</v>
       </c>
       <c r="D54" s="12"/>
@@ -1914,15 +1903,15 @@
         <v>67</v>
       </c>
       <c r="N54" s="12"/>
-      <c r="O54" s="27" t="s">
+      <c r="O54" s="28" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="22" t="s">
         <v>117</v>
       </c>
       <c r="D55" s="12"/>
@@ -1940,15 +1929,15 @@
         <v>68</v>
       </c>
       <c r="N55" s="12"/>
-      <c r="O55" s="27" t="s">
+      <c r="O55" s="28" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F56" s="9"/>
@@ -1957,10 +1946,10 @@
       <c r="M56" s="9"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="22" t="s">
         <v>119</v>
       </c>
       <c r="F57" s="9"/>
@@ -1969,10 +1958,10 @@
       <c r="M57" s="9"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F58" s="9"/>
@@ -1981,10 +1970,10 @@
       <c r="M58" s="9"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="22" t="s">
         <v>121</v>
       </c>
       <c r="F59" s="9"/>
@@ -1993,51 +1982,43 @@
       <c r="M59" s="9"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="22" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="27" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="27" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="27" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="27" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>